<commit_message>
Updated with new values using Mass replacement
</commit_message>
<xml_diff>
--- a/Mathematical Model/Simulation Results/TrimmerFunOutputs.xlsx
+++ b/Mathematical Model/Simulation Results/TrimmerFunOutputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camden\Desktop\Spring 2021\ECE 413\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E5426D-6B38-4EE3-9BE5-46E715A00037}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DACD233-9FF6-4282-A82B-4BE5BD180FF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3E7BA12B-8919-4C4C-84D9-B0F0175A724F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="35">
   <si>
     <t>State Vector</t>
   </si>
@@ -137,6 +137,9 @@
   <si>
     <t>10000 ft</t>
   </si>
+  <si>
+    <t>300 ft</t>
+  </si>
 </sst>
 </file>
 
@@ -162,18 +165,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -357,22 +354,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,9 +369,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,15 +410,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>88851</xdr:colOff>
+      <xdr:colOff>190499</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>589517</xdr:colOff>
+      <xdr:colOff>522840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>126338</xdr:rowOff>
+      <xdr:rowOff>41913</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -449,8 +446,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11118801" y="0"/>
-          <a:ext cx="5987066" cy="3002888"/>
+          <a:off x="11220449" y="1"/>
+          <a:ext cx="5818741" cy="2918462"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -462,15 +459,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>107364</xdr:rowOff>
+      <xdr:rowOff>107663</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>361948</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>7098</xdr:rowOff>
+      <xdr:rowOff>117276</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -499,8 +496,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11182349" y="12213639"/>
-          <a:ext cx="5934075" cy="2976309"/>
+          <a:off x="11334750" y="12213938"/>
+          <a:ext cx="6153148" cy="3086188"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -512,15 +509,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>237</xdr:rowOff>
+      <xdr:rowOff>105012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>166255</xdr:rowOff>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>71005</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -549,7 +546,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11144250" y="15383112"/>
+          <a:off x="11420475" y="15487887"/>
           <a:ext cx="5667376" cy="2842543"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -562,15 +559,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>182761</xdr:rowOff>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>77986</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>163711</xdr:rowOff>
+      <xdr:rowOff>168191</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -599,8 +596,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11125200" y="18242161"/>
-          <a:ext cx="6096000" cy="3057525"/>
+          <a:off x="11182349" y="18337411"/>
+          <a:ext cx="5915025" cy="2966755"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -651,6 +648,156 @@
         <a:xfrm>
           <a:off x="11172825" y="21672113"/>
           <a:ext cx="6019800" cy="3019306"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>103569</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>183594</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43EFB4E7-91C0-4F4E-BC17-DED5EDC6A719}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11229974" y="3180144"/>
+          <a:ext cx="5495925" cy="2756550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268629</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>59769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B91388DB-3585-4C68-9FDB-F1D2D4A5EB5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11298579" y="6210300"/>
+          <a:ext cx="5341596" cy="2679144"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>234563</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>78819</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3894C25F-A303-4914-80CB-6B5A1CFDC788}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11264513" y="9058275"/>
+          <a:ext cx="6632961" cy="3326844"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -962,7 +1109,7 @@
   <dimension ref="A1:K127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,55 +1128,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="15" t="s">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="15" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="12"/>
+      <c r="J1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="19"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="13"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1209,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1095,7 +1242,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1128,7 +1275,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1308,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1184,7 +1331,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1205,7 +1352,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1226,7 +1373,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1247,7 +1394,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1268,7 +1415,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1289,7 +1436,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1310,7 +1457,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1321,7 +1468,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>18</v>
@@ -1331,7 +1478,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1352,59 +1499,59 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="15" t="s">
+      <c r="B17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="15" t="s">
+      <c r="G17" s="13"/>
+      <c r="H17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="19"/>
+      <c r="K17" s="13"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="10" t="s">
+      <c r="G18" s="15"/>
+      <c r="H18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="12" t="s">
+      <c r="I18" s="17"/>
+      <c r="J18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="13"/>
+      <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
@@ -1437,7 +1584,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1460,17 +1607,17 @@
         <v>5</v>
       </c>
       <c r="I20" s="3">
-        <v>0.58280321095244703</v>
+        <v>3.8587835162712997E-2</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="9">
-        <v>8662.4408874599903</v>
+      <c r="K20" s="20">
+        <v>-6.8328530000000002E-9</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
@@ -1503,7 +1650,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
@@ -1536,7 +1683,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1555,11 +1702,11 @@
         <v>11</v>
       </c>
       <c r="I23" s="3">
-        <v>0.58280321095244703</v>
+        <v>3.8587835162712997E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1580,7 +1727,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="2" t="s">
         <v>13</v>
       </c>
@@ -1601,7 +1748,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="2" t="s">
         <v>14</v>
       </c>
@@ -1622,7 +1769,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="2" t="s">
         <v>15</v>
       </c>
@@ -1643,7 +1790,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="2" t="s">
         <v>16</v>
       </c>
@@ -1664,7 +1811,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
@@ -1685,7 +1832,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
@@ -1696,7 +1843,7 @@
         <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>18</v>
@@ -1706,7 +1853,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
@@ -1728,55 +1875,55 @@
     </row>
     <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="15" t="s">
+      <c r="B33" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I33" s="18"/>
-      <c r="J33" s="15" t="s">
+      <c r="G33" s="13"/>
+      <c r="H33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="12"/>
+      <c r="J33" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K33" s="19"/>
+      <c r="K33" s="13"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="12" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="10" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12" t="s">
+      <c r="E34" s="17"/>
+      <c r="F34" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="10" t="s">
+      <c r="G34" s="15"/>
+      <c r="H34" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I34" s="11"/>
-      <c r="J34" s="12" t="s">
+      <c r="I34" s="17"/>
+      <c r="J34" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K34" s="13"/>
+      <c r="K34" s="15"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
@@ -1809,7 +1956,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
@@ -1832,17 +1979,17 @@
         <v>5</v>
       </c>
       <c r="I36" s="3">
-        <v>0.78781812991877798</v>
+        <v>3.8612235910497998E-2</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K36" s="9">
-        <v>4349.9885957214701</v>
+      <c r="K36" s="20">
+        <v>6.8124000000000002E-11</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="2" t="s">
         <v>7</v>
       </c>
@@ -1871,11 +2018,11 @@
         <v>8</v>
       </c>
       <c r="K37" s="6">
-        <v>-0.34643273020900001</v>
+        <v>-7.8690929680169993E-3</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
@@ -1898,17 +2045,17 @@
         <v>9</v>
       </c>
       <c r="I38" s="3">
-        <v>2.2800666153660002E-3</v>
+        <v>3.2051237432210002E-3</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K38" s="7">
-        <v>-10.720135301003999</v>
+        <v>-4.4902790515962E-2</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="2" t="s">
         <v>11</v>
       </c>
@@ -1927,11 +2074,11 @@
         <v>11</v>
       </c>
       <c r="I39" s="3">
-        <v>0.78779211225035495</v>
+        <v>3.8610415281224997E-2</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="2" t="s">
         <v>12</v>
       </c>
@@ -1952,7 +2099,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
@@ -1973,7 +2120,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1994,7 +2141,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="2" t="s">
         <v>15</v>
       </c>
@@ -2015,7 +2162,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="2" t="s">
         <v>16</v>
       </c>
@@ -2036,7 +2183,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="2" t="s">
         <v>17</v>
       </c>
@@ -2057,7 +2204,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="2" t="s">
         <v>18</v>
       </c>
@@ -2068,7 +2215,7 @@
         <v>18</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>18</v>
@@ -2078,7 +2225,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
+      <c r="A47" s="18"/>
       <c r="B47" s="4" t="s">
         <v>20</v>
       </c>
@@ -2100,55 +2247,55 @@
     </row>
     <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="15" t="s">
+      <c r="B49" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="12"/>
+      <c r="F49" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I49" s="18"/>
-      <c r="J49" s="15" t="s">
+      <c r="G49" s="13"/>
+      <c r="H49" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" s="12"/>
+      <c r="J49" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K49" s="19"/>
+      <c r="K49" s="13"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="12" t="s">
+      <c r="A50" s="18"/>
+      <c r="B50" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="10" t="s">
+      <c r="C50" s="15"/>
+      <c r="D50" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="11"/>
-      <c r="F50" s="12" t="s">
+      <c r="E50" s="17"/>
+      <c r="F50" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G50" s="13"/>
-      <c r="H50" s="10" t="s">
+      <c r="G50" s="15"/>
+      <c r="H50" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I50" s="11"/>
-      <c r="J50" s="12" t="s">
+      <c r="I50" s="17"/>
+      <c r="J50" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K50" s="13"/>
+      <c r="K50" s="15"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
@@ -2181,7 +2328,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
@@ -2204,17 +2351,17 @@
         <v>5</v>
       </c>
       <c r="I52" s="3">
-        <v>0.58280321095244703</v>
+        <v>3.8587835162712997E-2</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K52" s="9">
-        <v>8662.4408874599903</v>
+      <c r="K52" s="20">
+        <v>-6.8328530000000002E-9</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
@@ -2247,7 +2394,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="14"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="2" t="s">
         <v>9</v>
       </c>
@@ -2280,7 +2427,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
@@ -2299,11 +2446,11 @@
         <v>11</v>
       </c>
       <c r="I55" s="3">
-        <v>0.58280321095244703</v>
+        <v>3.8587835162712997E-2</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
+      <c r="A56" s="18"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
@@ -2324,7 +2471,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="2" t="s">
         <v>13</v>
       </c>
@@ -2345,7 +2492,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="2" t="s">
         <v>14</v>
       </c>
@@ -2366,7 +2513,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="2" t="s">
         <v>15</v>
       </c>
@@ -2387,7 +2534,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="2" t="s">
         <v>16</v>
       </c>
@@ -2408,7 +2555,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="2" t="s">
         <v>17</v>
       </c>
@@ -2429,7 +2576,7 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="2" t="s">
         <v>18</v>
       </c>
@@ -2440,7 +2587,7 @@
         <v>18</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>18</v>
@@ -2450,7 +2597,7 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="14"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
@@ -2472,55 +2619,55 @@
     </row>
     <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="18"/>
-      <c r="F65" s="15" t="s">
+      <c r="B65" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="12"/>
+      <c r="F65" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G65" s="19"/>
-      <c r="H65" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I65" s="18"/>
-      <c r="J65" s="15" t="s">
+      <c r="G65" s="13"/>
+      <c r="H65" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I65" s="12"/>
+      <c r="J65" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K65" s="19"/>
+      <c r="K65" s="13"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="12" t="s">
+      <c r="A66" s="18"/>
+      <c r="B66" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="10" t="s">
+      <c r="C66" s="15"/>
+      <c r="D66" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E66" s="11"/>
-      <c r="F66" s="12" t="s">
+      <c r="E66" s="17"/>
+      <c r="F66" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G66" s="13"/>
-      <c r="H66" s="10" t="s">
+      <c r="G66" s="15"/>
+      <c r="H66" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I66" s="11"/>
-      <c r="J66" s="12" t="s">
+      <c r="I66" s="17"/>
+      <c r="J66" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K66" s="13"/>
+      <c r="K66" s="15"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="2" t="s">
         <v>2</v>
       </c>
@@ -2553,7 +2700,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="18"/>
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
@@ -2586,7 +2733,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="18"/>
       <c r="B69" s="2" t="s">
         <v>7</v>
       </c>
@@ -2619,7 +2766,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="14"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
@@ -2652,7 +2799,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="2" t="s">
         <v>11</v>
       </c>
@@ -2675,7 +2822,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="2" t="s">
         <v>12</v>
       </c>
@@ -2696,7 +2843,7 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="18"/>
       <c r="B73" s="2" t="s">
         <v>13</v>
       </c>
@@ -2717,7 +2864,7 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="18"/>
       <c r="B74" s="2" t="s">
         <v>14</v>
       </c>
@@ -2738,7 +2885,7 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="2" t="s">
         <v>15</v>
       </c>
@@ -2759,7 +2906,7 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="2" t="s">
         <v>16</v>
       </c>
@@ -2780,7 +2927,7 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="2" t="s">
         <v>17</v>
       </c>
@@ -2801,7 +2948,7 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="2" t="s">
         <v>18</v>
       </c>
@@ -2822,7 +2969,7 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="14"/>
+      <c r="A79" s="18"/>
       <c r="B79" s="4" t="s">
         <v>20</v>
       </c>
@@ -2844,55 +2991,55 @@
     </row>
     <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
+      <c r="A81" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B81" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="16"/>
-      <c r="D81" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="18"/>
-      <c r="F81" s="15" t="s">
+      <c r="B81" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="10"/>
+      <c r="D81" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="12"/>
+      <c r="F81" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G81" s="19"/>
-      <c r="H81" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I81" s="18"/>
-      <c r="J81" s="15" t="s">
+      <c r="G81" s="13"/>
+      <c r="H81" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I81" s="12"/>
+      <c r="J81" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K81" s="19"/>
+      <c r="K81" s="13"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="12" t="s">
+      <c r="A82" s="18"/>
+      <c r="B82" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C82" s="13"/>
-      <c r="D82" s="10" t="s">
+      <c r="C82" s="15"/>
+      <c r="D82" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E82" s="11"/>
-      <c r="F82" s="12" t="s">
+      <c r="E82" s="17"/>
+      <c r="F82" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G82" s="13"/>
-      <c r="H82" s="10" t="s">
+      <c r="G82" s="15"/>
+      <c r="H82" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I82" s="11"/>
-      <c r="J82" s="12" t="s">
+      <c r="I82" s="17"/>
+      <c r="J82" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K82" s="13"/>
+      <c r="K82" s="15"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="18"/>
       <c r="B83" s="2" t="s">
         <v>2</v>
       </c>
@@ -2925,7 +3072,7 @@
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="18"/>
       <c r="B84" s="2" t="s">
         <v>5</v>
       </c>
@@ -2958,7 +3105,7 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="18"/>
       <c r="B85" s="2" t="s">
         <v>7</v>
       </c>
@@ -2991,7 +3138,7 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="14"/>
+      <c r="A86" s="18"/>
       <c r="B86" s="2" t="s">
         <v>9</v>
       </c>
@@ -3024,7 +3171,7 @@
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="18"/>
       <c r="B87" s="2" t="s">
         <v>11</v>
       </c>
@@ -3047,7 +3194,7 @@
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="14"/>
+      <c r="A88" s="18"/>
       <c r="B88" s="2" t="s">
         <v>12</v>
       </c>
@@ -3068,7 +3215,7 @@
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="18"/>
       <c r="B89" s="2" t="s">
         <v>13</v>
       </c>
@@ -3089,7 +3236,7 @@
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="18"/>
       <c r="B90" s="2" t="s">
         <v>14</v>
       </c>
@@ -3110,7 +3257,7 @@
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
+      <c r="A91" s="18"/>
       <c r="B91" s="2" t="s">
         <v>15</v>
       </c>
@@ -3131,7 +3278,7 @@
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
+      <c r="A92" s="18"/>
       <c r="B92" s="2" t="s">
         <v>16</v>
       </c>
@@ -3152,7 +3299,7 @@
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="14"/>
+      <c r="A93" s="18"/>
       <c r="B93" s="2" t="s">
         <v>17</v>
       </c>
@@ -3173,7 +3320,7 @@
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="18"/>
       <c r="B94" s="2" t="s">
         <v>18</v>
       </c>
@@ -3194,7 +3341,7 @@
       </c>
     </row>
     <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="14"/>
+      <c r="A95" s="18"/>
       <c r="B95" s="4" t="s">
         <v>20</v>
       </c>
@@ -3216,55 +3363,55 @@
     </row>
     <row r="96" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
+      <c r="A97" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B97" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C97" s="16"/>
-      <c r="D97" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="18"/>
-      <c r="F97" s="15" t="s">
+      <c r="B97" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="10"/>
+      <c r="D97" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="12"/>
+      <c r="F97" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G97" s="19"/>
-      <c r="H97" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I97" s="18"/>
-      <c r="J97" s="15" t="s">
+      <c r="G97" s="13"/>
+      <c r="H97" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I97" s="12"/>
+      <c r="J97" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K97" s="19"/>
+      <c r="K97" s="13"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
-      <c r="B98" s="12" t="s">
+      <c r="A98" s="18"/>
+      <c r="B98" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C98" s="13"/>
-      <c r="D98" s="10" t="s">
+      <c r="C98" s="15"/>
+      <c r="D98" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E98" s="11"/>
-      <c r="F98" s="12" t="s">
+      <c r="E98" s="17"/>
+      <c r="F98" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G98" s="13"/>
-      <c r="H98" s="10" t="s">
+      <c r="G98" s="15"/>
+      <c r="H98" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I98" s="11"/>
-      <c r="J98" s="12" t="s">
+      <c r="I98" s="17"/>
+      <c r="J98" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K98" s="13"/>
+      <c r="K98" s="15"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
+      <c r="A99" s="18"/>
       <c r="B99" s="2" t="s">
         <v>2</v>
       </c>
@@ -3297,7 +3444,7 @@
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="18"/>
       <c r="B100" s="2" t="s">
         <v>5</v>
       </c>
@@ -3330,7 +3477,7 @@
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="14"/>
+      <c r="A101" s="18"/>
       <c r="B101" s="2" t="s">
         <v>7</v>
       </c>
@@ -3363,7 +3510,7 @@
       </c>
     </row>
     <row r="102" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="14"/>
+      <c r="A102" s="18"/>
       <c r="B102" s="2" t="s">
         <v>9</v>
       </c>
@@ -3396,7 +3543,7 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="18"/>
       <c r="B103" s="2" t="s">
         <v>11</v>
       </c>
@@ -3419,7 +3566,7 @@
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="18"/>
       <c r="B104" s="2" t="s">
         <v>12</v>
       </c>
@@ -3440,7 +3587,7 @@
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
+      <c r="A105" s="18"/>
       <c r="B105" s="2" t="s">
         <v>13</v>
       </c>
@@ -3461,7 +3608,7 @@
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
+      <c r="A106" s="18"/>
       <c r="B106" s="2" t="s">
         <v>14</v>
       </c>
@@ -3482,7 +3629,7 @@
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="14"/>
+      <c r="A107" s="18"/>
       <c r="B107" s="2" t="s">
         <v>15</v>
       </c>
@@ -3503,7 +3650,7 @@
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="14"/>
+      <c r="A108" s="18"/>
       <c r="B108" s="2" t="s">
         <v>16</v>
       </c>
@@ -3524,7 +3671,7 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="14"/>
+      <c r="A109" s="18"/>
       <c r="B109" s="2" t="s">
         <v>17</v>
       </c>
@@ -3545,7 +3692,7 @@
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="14"/>
+      <c r="A110" s="18"/>
       <c r="B110" s="2" t="s">
         <v>18</v>
       </c>
@@ -3566,7 +3713,7 @@
       </c>
     </row>
     <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="14"/>
+      <c r="A111" s="18"/>
       <c r="B111" s="4" t="s">
         <v>20</v>
       </c>
@@ -3588,55 +3735,55 @@
     </row>
     <row r="112" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="s">
+      <c r="A113" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B113" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C113" s="16"/>
-      <c r="D113" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E113" s="18"/>
-      <c r="F113" s="15" t="s">
+      <c r="B113" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="10"/>
+      <c r="D113" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E113" s="12"/>
+      <c r="F113" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G113" s="19"/>
-      <c r="H113" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I113" s="18"/>
-      <c r="J113" s="15" t="s">
+      <c r="G113" s="13"/>
+      <c r="H113" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I113" s="12"/>
+      <c r="J113" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K113" s="19"/>
+      <c r="K113" s="13"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
-      <c r="B114" s="12" t="s">
+      <c r="A114" s="18"/>
+      <c r="B114" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C114" s="13"/>
-      <c r="D114" s="10" t="s">
+      <c r="C114" s="15"/>
+      <c r="D114" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E114" s="11"/>
-      <c r="F114" s="12" t="s">
+      <c r="E114" s="17"/>
+      <c r="F114" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G114" s="13"/>
-      <c r="H114" s="10" t="s">
+      <c r="G114" s="15"/>
+      <c r="H114" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I114" s="11"/>
-      <c r="J114" s="12" t="s">
+      <c r="I114" s="17"/>
+      <c r="J114" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K114" s="13"/>
+      <c r="K114" s="15"/>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="18"/>
       <c r="B115" s="2" t="s">
         <v>2</v>
       </c>
@@ -3669,7 +3816,7 @@
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="18"/>
       <c r="B116" s="2" t="s">
         <v>5</v>
       </c>
@@ -3702,7 +3849,7 @@
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="14"/>
+      <c r="A117" s="18"/>
       <c r="B117" s="2" t="s">
         <v>7</v>
       </c>
@@ -3735,7 +3882,7 @@
       </c>
     </row>
     <row r="118" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="14"/>
+      <c r="A118" s="18"/>
       <c r="B118" s="2" t="s">
         <v>9</v>
       </c>
@@ -3768,7 +3915,7 @@
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="18"/>
       <c r="B119" s="2" t="s">
         <v>11</v>
       </c>
@@ -3791,7 +3938,7 @@
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="18"/>
       <c r="B120" s="2" t="s">
         <v>12</v>
       </c>
@@ -3812,7 +3959,7 @@
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="18"/>
       <c r="B121" s="2" t="s">
         <v>13</v>
       </c>
@@ -3833,7 +3980,7 @@
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="18"/>
       <c r="B122" s="2" t="s">
         <v>14</v>
       </c>
@@ -3854,7 +4001,7 @@
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="14"/>
+      <c r="A123" s="18"/>
       <c r="B123" s="2" t="s">
         <v>15</v>
       </c>
@@ -3875,7 +4022,7 @@
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
+      <c r="A124" s="18"/>
       <c r="B124" s="2" t="s">
         <v>16</v>
       </c>
@@ -3896,7 +4043,7 @@
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
+      <c r="A125" s="18"/>
       <c r="B125" s="2" t="s">
         <v>17</v>
       </c>
@@ -3917,7 +4064,7 @@
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
+      <c r="A126" s="18"/>
       <c r="B126" s="2" t="s">
         <v>18</v>
       </c>
@@ -3938,7 +4085,7 @@
       </c>
     </row>
     <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="14"/>
+      <c r="A127" s="18"/>
       <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
@@ -3960,11 +4107,74 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="J98:K98"/>
+    <mergeCell ref="A113:A127"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="F113:G113"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="A97:A111"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="F97:G97"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="J97:K97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="A81:A95"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="A65:A79"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="A49:A63"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A33:A47"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A17:A31"/>
@@ -3981,74 +4191,11 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A1:A15"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A33:A47"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A49:A63"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="A65:A79"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="A81:A95"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="J97:K97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="F98:G98"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J98:K98"/>
-    <mergeCell ref="A113:A127"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="F113:G113"/>
-    <mergeCell ref="H113:I113"/>
-    <mergeCell ref="J113:K113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="F114:G114"/>
-    <mergeCell ref="A97:A111"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="F97:G97"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>